<commit_message>
resume template, dynamic update
</commit_message>
<xml_diff>
--- a/scripts/resume-data-template.xlsx
+++ b/scripts/resume-data-template.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrose/proto/aws-serverless-resume/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrose/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54AF7B9-1651-644A-BFC8-1763C4678EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F6168-CD79-5849-9602-3206822601C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73700" yWindow="4720" windowWidth="23360" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="600" windowWidth="67640" windowHeight="28200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="WorkExperience" sheetId="2" r:id="rId2"/>
-    <sheet name="Education" sheetId="3" r:id="rId3"/>
-    <sheet name="Skills" sheetId="4" r:id="rId4"/>
+    <sheet name="Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="WorkExperience" sheetId="3" r:id="rId3"/>
+    <sheet name="Education" sheetId="4" r:id="rId4"/>
+    <sheet name="Skills" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Resume Data Entry Template</t>
   </si>
@@ -109,6 +110,66 @@
     <t>Technical and professional skills by category</t>
   </si>
   <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>your.email@example.com</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Sometown, IL</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>/assets/profile.jpg</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>Use this section to provide a brief summary about yourself, your skills, and your career objectives.</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>https://github.com/yoursite</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>https://linkedin.com/in/yoursite</t>
+  </si>
+  <si>
+    <t>resume_pdf</t>
+  </si>
+  <si>
+    <t>/assets/resume.pdf</t>
+  </si>
+  <si>
+    <t>professional_summary</t>
+  </si>
+  <si>
+    <t>Add a more detailed professional summary here. This will appear in a separate box on your About page.</t>
+  </si>
+  <si>
     <t>job_title</t>
   </si>
   <si>
@@ -214,22 +275,10 @@
     <t>FastAPI|React|Node.js|Git|CI/CD</t>
   </si>
   <si>
-    <t>Master of Science</t>
-  </si>
-  <si>
-    <t>Iowa State</t>
-  </si>
-  <si>
-    <t>2020-09</t>
-  </si>
-  <si>
-    <t>2022-05</t>
-  </si>
-  <si>
-    <t>Im good</t>
-  </si>
-  <si>
-    <t>2014-06</t>
+    <t>Rob Rose</t>
+  </si>
+  <si>
+    <t>Engineer</t>
   </si>
 </sst>
 </file>
@@ -749,11 +798,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -765,91 +919,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -857,13 +988,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -875,53 +1004,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -929,8 +1041,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -944,21 +1056,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -966,10 +1078,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -977,10 +1089,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>3</v>

</xml_diff>

<commit_message>
Add RAG embeddings infrastructure
- Configure LocalStack persistence for DynamoDB data
- Create ChatbotRAG table on startup
- Generate embeddings script with smart skip logic
- Prevent unnecessary OpenAI API calls on restart
</commit_message>
<xml_diff>
--- a/scripts/resume-data-template.xlsx
+++ b/scripts/resume-data-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrose/proto/aws-serverless-resume/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BFD009-65D0-BC4E-9ED6-126DE3E06AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73240832-0918-D245-9F0A-547803DF8F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73380" yWindow="7800" windowWidth="33820" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73380" yWindow="7800" windowWidth="33820" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>Resume Data Entry Template</t>
   </si>
@@ -231,12 +231,6 @@
   </si>
   <si>
     <t>State University</t>
-  </si>
-  <si>
-    <t>2014-09</t>
-  </si>
-  <si>
-    <t>2018-05</t>
   </si>
   <si>
     <t>GPA: 3.8/4.0, Dean's List, Computer Science Club President</t>
@@ -797,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -820,7 +814,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -828,7 +822,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -849,7 +843,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -986,7 +980,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1020,14 +1016,8 @@
       <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1050,21 +1040,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1072,10 +1062,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1083,10 +1073,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>3</v>

</xml_diff>

<commit_message>
experienceCleanUp: Minor housekeeping on some formatting and adding some things for additional experience
</commit_message>
<xml_diff>
--- a/scripts/resume-data-template.xlsx
+++ b/scripts/resume-data-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrose/proto/aws-serverless-resume/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73240832-0918-D245-9F0A-547803DF8F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EA3152-7B12-794A-9906-21EC9B9FE28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73380" yWindow="7800" windowWidth="33820" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73380" yWindow="7800" windowWidth="33820" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Resume Data Entry Template</t>
   </si>
@@ -270,13 +270,28 @@
   </si>
   <si>
     <t>/assets/profile.png</t>
+  </si>
+  <si>
+    <t>is_additional</t>
+  </si>
+  <si>
+    <t>My First job</t>
+  </si>
+  <si>
+    <t>Doesn’t matter</t>
+  </si>
+  <si>
+    <t>2016-01</t>
+  </si>
+  <si>
+    <t>2018-05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +320,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -332,13 +354,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,19 +916,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="25" customWidth="1"/>
     <col min="3" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -922,13 +947,16 @@
         <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -941,14 +969,17 @@
       <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -964,12 +995,47 @@
       <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>64</v>
       </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -980,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>